<commit_message>
fix delete attendee option
</commit_message>
<xml_diff>
--- a/public/templates/TeamClassAttendeesTemplate.xlsx
+++ b/public/templates/TeamClassAttendeesTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Documents\teamClassPortal\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Documents\teamclass\teamClassPortal\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDDC4DB-03AF-4972-9341-29560FA37F95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E35D5F-BAEB-40BE-89A4-8DC8EFB1E392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{32CF8B38-6F04-4898-A57E-6018B9997318}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Name</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Zip</t>
   </si>
   <si>
-    <t>Dietary Restrictions</t>
-  </si>
-  <si>
     <t>345 AV 38</t>
   </si>
   <si>
@@ -94,9 +91,6 @@
   </si>
   <si>
     <t>Miami</t>
-  </si>
-  <si>
-    <t>No sea food</t>
   </si>
 </sst>
 </file>
@@ -460,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E97BF38A-9C69-4904-831C-73D512BAE33C}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -478,7 +472,7 @@
     <col min="10" max="10" width="16.05078125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -506,11 +500,8 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -521,54 +512,51 @@
         <v>3182896543</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2">
         <v>30</v>
       </c>
       <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
         <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
       </c>
       <c r="H2">
         <v>10004</v>
       </c>
       <c r="I2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
+      <c r="B3" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="C3" s="1">
         <v>3142896543</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3">
         <v>50</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H3">
         <v>10004</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>